<commit_message>
Updates expenses to add number working for 2 adult families
</commit_message>
<xml_diff>
--- a/addison_county_101/storymap_data/expenses_county.xlsx
+++ b/addison_county_101/storymap_data/expenses_county.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrence/Documents/GitHub/privilege_and_poverty/addison_county_101/storymap_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF59DEF6-2375-5849-9CF9-BCA407CADC3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98C0E01-EF97-634A-B43E-FF7CEF2BAFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="1580" windowWidth="15820" windowHeight="13640" xr2:uid="{F7A4D10A-304E-2D47-B0AF-70C3F3FAF73F}"/>
+    <workbookView xWindow="180" yWindow="1580" windowWidth="24320" windowHeight="13820" xr2:uid="{F7A4D10A-304E-2D47-B0AF-70C3F3FAF73F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t>Food</t>
   </si>
@@ -99,6 +99,24 @@
   </si>
   <si>
     <t>Children</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Working Full-Time</t>
+  </si>
+  <si>
+    <t>1 Working Full-Time</t>
+  </si>
+  <si>
+    <t>Both Working Full-Time</t>
+  </si>
+  <si>
+    <t>Gain not gap</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -481,7 +499,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A7FF57-4E4B-C441-9C00-37FB60C178BD}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -492,16 +510,17 @@
   <cols>
     <col min="1" max="1" width="57.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.83203125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="85">
+    <row r="1" spans="1:18" ht="85">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -509,253 +528,271 @@
         <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="R1" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="68">
+    <row r="2" spans="1:18" ht="85">
       <c r="A2" s="4" t="str">
-        <f>_xlfn.CONCAT("A family with ", B2, " and ", C2, " would require $", L2, " to earn a living wage. Working at minimum wage would leave a gap of $", P2, ". A family at the poverty level would need an additional $", N2, " to have the income required for a living wage.")</f>
+        <f>_xlfn.CONCAT("A family with ", B2, " and ", D2, " would require $", M2, " to earn a living wage. Working at minimum wage would leave a gap of $", Q2, ". A family at the poverty level would need an additional $", O2, " to have the income required for a living wage.")</f>
         <v>A family with 1 adult and 0 children would require $24988 to earn a living wage. Working at minimum wage would leave a gap of $2565.6. A family at the poverty level would need an additional $12508 to have the income required for a living wage.</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="7">
+      <c r="E2" s="7">
         <v>3495</v>
       </c>
-      <c r="E2" s="7">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="F2" s="7">
+      <c r="G2" s="7">
         <v>2469</v>
       </c>
-      <c r="G2" s="7">
+      <c r="H2" s="7">
         <v>8472</v>
       </c>
-      <c r="H2" s="7">
+      <c r="I2" s="7">
         <v>3899</v>
       </c>
-      <c r="I2" s="7">
+      <c r="J2" s="7">
         <v>2890</v>
       </c>
-      <c r="J2" s="7">
+      <c r="K2" s="7">
         <v>21226</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="7">
         <v>3762</v>
       </c>
-      <c r="L2" s="7">
+      <c r="M2" s="7">
         <v>24988</v>
       </c>
-      <c r="M2" s="6">
+      <c r="N2" s="6">
         <v>12480</v>
       </c>
-      <c r="N2" s="6">
+      <c r="O2" s="6">
         <v>12508</v>
       </c>
-      <c r="O2" s="6">
+      <c r="P2" s="6">
         <v>22422.399999999998</v>
       </c>
-      <c r="P2" s="6">
+      <c r="Q2" s="6">
         <v>2565.6000000000022</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="68">
+    <row r="3" spans="1:18" ht="85">
       <c r="A3" s="4" t="str">
-        <f t="shared" ref="A3:A9" si="0">_xlfn.CONCAT("A family with ", B3, " and ", C3, " would require $", L3, " to earn a living wage. Working at minimum wage would leave a gap of $", P3, ". A family at the poverty level would need an additional $", N3, " to have the income required for a living wage.")</f>
+        <f t="shared" ref="A3:A13" si="0">_xlfn.CONCAT("A family with ", B3, " and ", D3, " would require $", M3, " to earn a living wage. Working at minimum wage would leave a gap of $", Q3, ". A family at the poverty level would need an additional $", O3, " to have the income required for a living wage.")</f>
         <v>A family with 1 adult and 1 child would require $53518 to earn a living wage. Working at minimum wage would leave a gap of $31095.6. A family at the poverty level would need an additional $36607.6 to have the income required for a living wage.</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="7">
+      <c r="E3" s="7">
         <v>5163</v>
       </c>
-      <c r="E3" s="7">
+      <c r="F3" s="7">
         <v>8235</v>
       </c>
-      <c r="F3" s="7">
+      <c r="G3" s="7">
         <v>7321</v>
       </c>
-      <c r="G3" s="7">
+      <c r="H3" s="7">
         <v>12072</v>
       </c>
-      <c r="H3" s="7">
+      <c r="I3" s="7">
         <v>7602</v>
       </c>
-      <c r="I3" s="7">
+      <c r="J3" s="7">
         <v>4818</v>
       </c>
-      <c r="J3" s="7">
+      <c r="K3" s="7">
         <v>45211</v>
       </c>
-      <c r="K3" s="7">
+      <c r="L3" s="7">
         <v>8307</v>
       </c>
-      <c r="L3" s="7">
+      <c r="M3" s="7">
         <v>53518</v>
       </c>
-      <c r="M3" s="6">
+      <c r="N3" s="6">
         <v>16910.400000000001</v>
       </c>
-      <c r="N3" s="6">
+      <c r="O3" s="6">
         <v>36607.599999999999</v>
       </c>
-      <c r="O3" s="6">
+      <c r="P3" s="6">
         <v>22422.399999999998</v>
       </c>
-      <c r="P3" s="6">
+      <c r="Q3" s="6">
         <v>31095.600000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="68">
+    <row r="4" spans="1:18" ht="85">
       <c r="A4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>A family with 1 adult and 2 children would require $63418 to earn a living wage. Working at minimum wage would leave a gap of $40995.6. A family at the poverty level would need an additional $42098 to have the income required for a living wage.</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7">
+      <c r="E4" s="7">
         <v>7760</v>
       </c>
-      <c r="E4" s="7">
+      <c r="F4" s="7">
         <v>11898</v>
       </c>
-      <c r="F4" s="7">
+      <c r="G4" s="7">
         <v>7033</v>
       </c>
-      <c r="G4" s="7">
+      <c r="H4" s="7">
         <v>12072</v>
       </c>
-      <c r="H4" s="7">
+      <c r="I4" s="7">
         <v>9644</v>
       </c>
-      <c r="I4" s="7">
+      <c r="J4" s="7">
         <v>5003</v>
       </c>
-      <c r="J4" s="7">
+      <c r="K4" s="7">
         <v>53409</v>
       </c>
-      <c r="K4" s="7">
+      <c r="L4" s="7">
         <v>10008</v>
       </c>
-      <c r="L4" s="7">
+      <c r="M4" s="7">
         <v>63418</v>
       </c>
-      <c r="M4" s="6">
+      <c r="N4" s="6">
         <v>21320</v>
       </c>
-      <c r="N4" s="6">
+      <c r="O4" s="6">
         <v>42098</v>
       </c>
-      <c r="O4" s="6">
+      <c r="P4" s="6">
         <v>22422.399999999998</v>
       </c>
-      <c r="P4" s="6">
+      <c r="Q4" s="6">
         <v>40995.600000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="68">
+    <row r="5" spans="1:18" ht="85">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>A family with 1 adult and 3 children would require $77425 to earn a living wage. Working at minimum wage would leave a gap of $55002.6. A family at the poverty level would need an additional $51674.6 to have the income required for a living wage.</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="7">
+      <c r="E5" s="7">
         <v>10292</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="7">
         <v>15560</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="7">
         <v>7153</v>
       </c>
-      <c r="G5" s="7">
+      <c r="H5" s="7">
         <v>15144</v>
       </c>
-      <c r="H5" s="7">
+      <c r="I5" s="7">
         <v>10506</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="7">
         <v>6293</v>
       </c>
-      <c r="J5" s="7">
+      <c r="K5" s="7">
         <v>64949</v>
       </c>
-      <c r="K5" s="7">
+      <c r="L5" s="7">
         <v>12476</v>
       </c>
-      <c r="L5" s="7">
+      <c r="M5" s="7">
         <v>77425</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="6">
         <v>25750.400000000001</v>
       </c>
-      <c r="N5" s="6">
+      <c r="O5" s="6">
         <v>51674.6</v>
       </c>
-      <c r="O5" s="6">
+      <c r="P5" s="6">
         <v>22422.399999999998</v>
       </c>
-      <c r="P5" s="6">
+      <c r="Q5" s="6">
         <v>55002.600000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="68">
+    <row r="6" spans="1:18" ht="85">
       <c r="A6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>A family with 2 adults and 0 children would require $40670 to earn a living wage. Working at minimum wage would leave a gap of $18247.6. A family at the poverty level would need an additional $23759.6 to have the income required for a living wage.</v>
@@ -764,100 +801,106 @@
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E6" s="7">
         <v>6408</v>
       </c>
-      <c r="E6" s="7">
+      <c r="F6" s="7">
         <v>0</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="7">
         <v>5464</v>
       </c>
-      <c r="G6" s="7">
+      <c r="H6" s="7">
         <v>10296</v>
       </c>
-      <c r="H6" s="7">
+      <c r="I6" s="7">
         <v>7602</v>
       </c>
-      <c r="I6" s="7">
+      <c r="J6" s="7">
         <v>4818</v>
       </c>
-      <c r="J6" s="7">
+      <c r="K6" s="7">
         <v>34588</v>
       </c>
-      <c r="K6" s="7">
+      <c r="L6" s="7">
         <v>6082</v>
       </c>
-      <c r="L6" s="7">
+      <c r="M6" s="7">
         <v>40670</v>
       </c>
-      <c r="M6" s="6">
+      <c r="N6" s="6">
         <v>16910.400000000001</v>
       </c>
-      <c r="N6" s="6">
+      <c r="O6" s="6">
         <v>23759.599999999999</v>
       </c>
-      <c r="O6" s="6">
+      <c r="P6" s="6">
         <v>22422.399999999998</v>
       </c>
-      <c r="P6" s="6">
+      <c r="Q6" s="6">
         <v>18247.600000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="68">
+    <row r="7" spans="1:18" ht="85">
       <c r="A7" s="4" t="str">
-        <f>_xlfn.CONCAT("A family with ", B7, " and ", C7, " would require $", L7, " to earn a living wage. Working at minimum wage would leave a gap of $", P7, ". A family at the poverty level would need an additional $", N7, " to have the income required for a living wage.")</f>
+        <f>_xlfn.CONCAT("A family with ", B7, " and ", D7, " would require $", M7, " to earn a living wage. Working at minimum wage would leave a gap of $", Q7, ". A family at the poverty level would need an additional $", O7, " to have the income required for a living wage.")</f>
         <v>A family with 2 adults and 1 child would require $49325 to earn a living wage. Working at minimum wage would leave a gap of $26902.6. A family at the poverty level would need an additional $28005 to have the income required for a living wage.</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7">
+      <c r="E7" s="7">
         <v>7987</v>
       </c>
-      <c r="E7" s="7">
+      <c r="F7" s="7">
         <v>0</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="7">
         <v>7033</v>
       </c>
-      <c r="G7" s="7">
+      <c r="H7" s="7">
         <v>12072</v>
       </c>
-      <c r="H7" s="7">
+      <c r="I7" s="7">
         <v>9644</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="7">
         <v>5003</v>
       </c>
-      <c r="J7" s="7">
+      <c r="K7" s="7">
         <v>41738</v>
       </c>
-      <c r="K7" s="7">
+      <c r="L7" s="7">
         <v>7586</v>
       </c>
-      <c r="L7" s="7">
+      <c r="M7" s="7">
         <v>49325</v>
       </c>
-      <c r="M7" s="6">
+      <c r="N7" s="6">
         <v>21320</v>
       </c>
-      <c r="N7" s="6">
+      <c r="O7" s="6">
         <v>28005</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="6">
         <v>22422.399999999998</v>
       </c>
-      <c r="P7" s="6">
+      <c r="Q7" s="6">
         <v>26902.600000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="68">
+    <row r="8" spans="1:18" ht="85">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>A family with 2 adults and 2 children would require $54866 to earn a living wage. Working at minimum wage would leave a gap of $32443.6. A family at the poverty level would need an additional $29115.6 to have the income required for a living wage.</v>
@@ -866,49 +909,52 @@
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E8" s="7">
         <v>10303</v>
       </c>
-      <c r="E8" s="7">
+      <c r="F8" s="7">
         <v>0</v>
       </c>
-      <c r="F8" s="7">
+      <c r="G8" s="7">
         <v>7153</v>
       </c>
-      <c r="G8" s="7">
+      <c r="H8" s="7">
         <v>12072</v>
       </c>
-      <c r="H8" s="7">
+      <c r="I8" s="7">
         <v>10506</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="7">
         <v>6293</v>
       </c>
-      <c r="J8" s="7">
+      <c r="K8" s="7">
         <v>46328</v>
       </c>
-      <c r="K8" s="7">
+      <c r="L8" s="7">
         <v>8539</v>
       </c>
-      <c r="L8" s="7">
+      <c r="M8" s="7">
         <v>54866</v>
       </c>
-      <c r="M8" s="6">
+      <c r="N8" s="6">
         <v>25750.400000000001</v>
       </c>
-      <c r="N8" s="6">
+      <c r="O8" s="6">
         <v>29115.599999999999</v>
       </c>
-      <c r="O8" s="6">
+      <c r="P8" s="6">
         <v>22422.399999999998</v>
       </c>
-      <c r="P8" s="6">
+      <c r="Q8" s="6">
         <v>32443.600000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="68">
+    <row r="9" spans="1:18" ht="85">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>A family with 2 adults and 3 children would require $61853 to earn a living wage. Working at minimum wage would leave a gap of $39430.6. A family at the poverty level would need an additional $31693 to have the income required for a living wage.</v>
@@ -917,46 +963,272 @@
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7">
+      <c r="E9" s="7">
         <v>12545</v>
       </c>
-      <c r="E9" s="7">
+      <c r="F9" s="7">
         <v>0</v>
       </c>
-      <c r="F9" s="7">
+      <c r="G9" s="7">
         <v>7055</v>
       </c>
-      <c r="G9" s="7">
+      <c r="H9" s="7">
         <v>15144</v>
       </c>
-      <c r="H9" s="7">
+      <c r="I9" s="7">
         <v>11013</v>
       </c>
-      <c r="I9" s="7">
+      <c r="J9" s="7">
         <v>6296</v>
       </c>
-      <c r="J9" s="7">
+      <c r="K9" s="7">
         <v>52052</v>
       </c>
-      <c r="K9" s="7">
+      <c r="L9" s="7">
         <v>9800</v>
       </c>
-      <c r="L9" s="7">
+      <c r="M9" s="7">
         <v>61853</v>
       </c>
-      <c r="M9" s="6">
+      <c r="N9" s="6">
         <v>30160</v>
       </c>
-      <c r="N9" s="6">
+      <c r="O9" s="6">
         <v>31693</v>
       </c>
-      <c r="O9" s="6">
+      <c r="P9" s="6">
         <v>22422.399999999998</v>
       </c>
-      <c r="P9" s="6">
+      <c r="Q9" s="6">
         <v>39430.600000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="85">
+      <c r="A10" s="4" t="str">
+        <f>_xlfn.CONCAT("A family with ", B10, " and ", D10, " would require $", M10, " to earn a living wage. Working at minimum wage would provide a living wage with savings of $", Q10, ". A family at the poverty level would need an additional $", O10, " to have the income required for a living wage.")</f>
+        <v>A family with 2 adults and 0 children would require $40670 to earn a living wage. Working at minimum wage would provide a living wage with savings of $4174.8. A family at the poverty level would need an additional $23759.6 to have the income required for a living wage.</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="7">
+        <v>6408</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>5464</v>
+      </c>
+      <c r="H10" s="7">
+        <v>10296</v>
+      </c>
+      <c r="I10" s="7">
+        <v>7602</v>
+      </c>
+      <c r="J10" s="7">
+        <v>4818</v>
+      </c>
+      <c r="K10" s="7">
+        <v>34588</v>
+      </c>
+      <c r="L10" s="7">
+        <v>6082</v>
+      </c>
+      <c r="M10" s="7">
+        <v>40670</v>
+      </c>
+      <c r="N10" s="6">
+        <v>16910.400000000001</v>
+      </c>
+      <c r="O10" s="6">
+        <v>23759.599999999999</v>
+      </c>
+      <c r="P10" s="6">
+        <v>44844.800000000003</v>
+      </c>
+      <c r="Q10" s="7">
+        <f>P10-M10</f>
+        <v>4174.8000000000029</v>
+      </c>
+      <c r="R10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="85">
+      <c r="A11" s="4" t="str">
+        <f>_xlfn.CONCAT("A family with ", B11, " and ", D11, " would require $", M11, " to earn a living wage. Working at minimum wage would leave a gap of $", Q11, ". A family at the poverty level would need an additional $", O11, " to have the income required for a living wage.")</f>
+        <v>A family with 2 adults and 1 child would require $49325 to earn a living wage. Working at minimum wage would leave a gap of $4480.2. A family at the poverty level would need an additional $28005 to have the income required for a living wage.</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="7">
+        <v>7987</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <v>7033</v>
+      </c>
+      <c r="H11" s="7">
+        <v>12072</v>
+      </c>
+      <c r="I11" s="7">
+        <v>9644</v>
+      </c>
+      <c r="J11" s="7">
+        <v>5003</v>
+      </c>
+      <c r="K11" s="7">
+        <v>41738</v>
+      </c>
+      <c r="L11" s="7">
+        <v>7586</v>
+      </c>
+      <c r="M11" s="7">
+        <v>49325</v>
+      </c>
+      <c r="N11" s="6">
+        <v>21320</v>
+      </c>
+      <c r="O11" s="6">
+        <v>28005</v>
+      </c>
+      <c r="P11" s="6">
+        <v>44844.800000000003</v>
+      </c>
+      <c r="Q11" s="7">
+        <f t="shared" ref="Q11:Q13" si="1">M11 - P11</f>
+        <v>4480.1999999999971</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="85">
+      <c r="A12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>A family with 2 adults and 2 children would require $54866 to earn a living wage. Working at minimum wage would leave a gap of $10021.2. A family at the poverty level would need an additional $29115.6 to have the income required for a living wage.</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="7">
+        <v>10303</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7">
+        <v>7153</v>
+      </c>
+      <c r="H12" s="7">
+        <v>12072</v>
+      </c>
+      <c r="I12" s="7">
+        <v>10506</v>
+      </c>
+      <c r="J12" s="7">
+        <v>6293</v>
+      </c>
+      <c r="K12" s="7">
+        <v>46328</v>
+      </c>
+      <c r="L12" s="7">
+        <v>8539</v>
+      </c>
+      <c r="M12" s="7">
+        <v>54866</v>
+      </c>
+      <c r="N12" s="6">
+        <v>25750.400000000001</v>
+      </c>
+      <c r="O12" s="6">
+        <v>29115.599999999999</v>
+      </c>
+      <c r="P12" s="6">
+        <v>44844.800000000003</v>
+      </c>
+      <c r="Q12" s="7">
+        <f t="shared" si="1"/>
+        <v>10021.199999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="85">
+      <c r="A13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>A family with 2 adults and 3 children would require $61853 to earn a living wage. Working at minimum wage would leave a gap of $17008.2. A family at the poverty level would need an additional $31693 to have the income required for a living wage.</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="7">
+        <v>12545</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>7055</v>
+      </c>
+      <c r="H13" s="7">
+        <v>15144</v>
+      </c>
+      <c r="I13" s="7">
+        <v>11013</v>
+      </c>
+      <c r="J13" s="7">
+        <v>6296</v>
+      </c>
+      <c r="K13" s="7">
+        <v>52052</v>
+      </c>
+      <c r="L13" s="7">
+        <v>9800</v>
+      </c>
+      <c r="M13" s="7">
+        <v>61853</v>
+      </c>
+      <c r="N13" s="6">
+        <v>30160</v>
+      </c>
+      <c r="O13" s="6">
+        <v>31693</v>
+      </c>
+      <c r="P13" s="6">
+        <v>44844.800000000003</v>
+      </c>
+      <c r="Q13" s="7">
+        <f t="shared" si="1"/>
+        <v>17008.199999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates expenses with child care and taxes for 2 adults both working
</commit_message>
<xml_diff>
--- a/addison_county_101/storymap_data/expenses_county.xlsx
+++ b/addison_county_101/storymap_data/expenses_county.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrence/Documents/GitHub/privilege_and_poverty/addison_county_101/storymap_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98C0E01-EF97-634A-B43E-FF7CEF2BAFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8BB877-C10F-9848-9BBF-E0DF9C3B57E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="1580" windowWidth="24320" windowHeight="13820" xr2:uid="{F7A4D10A-304E-2D47-B0AF-70C3F3FAF73F}"/>
+    <workbookView xWindow="26860" yWindow="-860" windowWidth="34640" windowHeight="17240" xr2:uid="{F7A4D10A-304E-2D47-B0AF-70C3F3FAF73F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +142,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF32474F"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF32474F"/>
       <name val="Helvetica"/>
       <family val="2"/>
@@ -167,22 +173,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -503,732 +519,772 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD1048576"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="57.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.83203125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="6" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="85">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="85">
-      <c r="A2" s="4" t="str">
+    <row r="2" spans="1:18" ht="68">
+      <c r="A2" s="2" t="str">
         <f>_xlfn.CONCAT("A family with ", B2, " and ", D2, " would require $", M2, " to earn a living wage. Working at minimum wage would leave a gap of $", Q2, ". A family at the poverty level would need an additional $", O2, " to have the income required for a living wage.")</f>
-        <v>A family with 1 adult and 0 children would require $24988 to earn a living wage. Working at minimum wage would leave a gap of $2565.6. A family at the poverty level would need an additional $12508 to have the income required for a living wage.</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>A family with 1 adult and 0 children would require $24987 to earn a living wage. Working at minimum wage would leave a gap of $2564.6. A family at the poverty level would need an additional $12507 to have the income required for a living wage.</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="8">
         <v>3495</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="8">
         <v>0</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="8">
         <v>2469</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="8">
         <v>8472</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="8">
         <v>3899</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="8">
         <v>2890</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="8">
         <v>21226</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="8">
         <v>3762</v>
       </c>
-      <c r="M2" s="7">
-        <v>24988</v>
-      </c>
-      <c r="N2" s="6">
+      <c r="M2" s="8">
+        <f>SUM(E2:J2) +  L2</f>
+        <v>24987</v>
+      </c>
+      <c r="N2" s="10">
         <v>12480</v>
       </c>
-      <c r="O2" s="6">
-        <v>12508</v>
-      </c>
-      <c r="P2" s="6">
+      <c r="O2" s="10">
+        <f>M2-N2</f>
+        <v>12507</v>
+      </c>
+      <c r="P2" s="10">
         <v>22422.399999999998</v>
       </c>
-      <c r="Q2" s="6">
-        <v>2565.6000000000022</v>
+      <c r="Q2" s="10">
+        <f>M2-P2</f>
+        <v>2564.6000000000022</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="85">
-      <c r="A3" s="4" t="str">
+    <row r="3" spans="1:18" ht="68">
+      <c r="A3" s="2" t="str">
         <f t="shared" ref="A3:A13" si="0">_xlfn.CONCAT("A family with ", B3, " and ", D3, " would require $", M3, " to earn a living wage. Working at minimum wage would leave a gap of $", Q3, ". A family at the poverty level would need an additional $", O3, " to have the income required for a living wage.")</f>
         <v>A family with 1 adult and 1 child would require $53518 to earn a living wage. Working at minimum wage would leave a gap of $31095.6. A family at the poverty level would need an additional $36607.6 to have the income required for a living wage.</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="8">
         <v>5163</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="8">
         <v>8235</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="8">
         <v>7321</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="8">
         <v>12072</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="8">
         <v>7602</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="8">
         <v>4818</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="8">
         <v>45211</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="8">
         <v>8307</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="8">
+        <f t="shared" ref="M3:M13" si="1">SUM(E3:J3) +  L3</f>
         <v>53518</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="10">
         <v>16910.400000000001</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="10">
+        <f t="shared" ref="O3:O13" si="2">M3-N3</f>
         <v>36607.599999999999</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="10">
         <v>22422.399999999998</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q3" s="10">
+        <f t="shared" ref="Q3:Q13" si="3">M3-P3</f>
         <v>31095.600000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="85">
-      <c r="A4" s="4" t="str">
+    <row r="4" spans="1:18" ht="68">
+      <c r="A4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>A family with 1 adult and 2 children would require $63418 to earn a living wage. Working at minimum wage would leave a gap of $40995.6. A family at the poverty level would need an additional $42098 to have the income required for a living wage.</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="8">
         <v>7760</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="8">
         <v>11898</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="8">
         <v>7033</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="8">
         <v>12072</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="8">
         <v>9644</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="8">
         <v>5003</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="8">
         <v>53409</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="8">
         <v>10008</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="8">
+        <f t="shared" si="1"/>
         <v>63418</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="10">
         <v>21320</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="10">
+        <f t="shared" si="2"/>
         <v>42098</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="10">
         <v>22422.399999999998</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="10">
+        <f t="shared" si="3"/>
         <v>40995.600000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="85">
-      <c r="A5" s="4" t="str">
+    <row r="5" spans="1:18" ht="68">
+      <c r="A5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>A family with 1 adult and 3 children would require $77425 to earn a living wage. Working at minimum wage would leave a gap of $55002.6. A family at the poverty level would need an additional $51674.6 to have the income required for a living wage.</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>A family with 1 adult and 3 children would require $77424 to earn a living wage. Working at minimum wage would leave a gap of $55001.6. A family at the poverty level would need an additional $51673.6 to have the income required for a living wage.</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="8">
         <v>10292</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="8">
         <v>15560</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="8">
         <v>7153</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="8">
         <v>15144</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="8">
         <v>10506</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="8">
         <v>6293</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="8">
         <v>64949</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="8">
         <v>12476</v>
       </c>
-      <c r="M5" s="7">
-        <v>77425</v>
-      </c>
-      <c r="N5" s="6">
+      <c r="M5" s="8">
+        <f t="shared" si="1"/>
+        <v>77424</v>
+      </c>
+      <c r="N5" s="10">
         <v>25750.400000000001</v>
       </c>
-      <c r="O5" s="6">
-        <v>51674.6</v>
-      </c>
-      <c r="P5" s="6">
+      <c r="O5" s="10">
+        <f t="shared" si="2"/>
+        <v>51673.599999999999</v>
+      </c>
+      <c r="P5" s="10">
         <v>22422.399999999998</v>
       </c>
-      <c r="Q5" s="6">
-        <v>55002.600000000006</v>
+      <c r="Q5" s="10">
+        <f t="shared" si="3"/>
+        <v>55001.600000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="85">
-      <c r="A6" s="4" t="str">
+    <row r="6" spans="1:18" ht="68">
+      <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>A family with 2 adults and 0 children would require $40670 to earn a living wage. Working at minimum wage would leave a gap of $18247.6. A family at the poverty level would need an additional $23759.6 to have the income required for a living wage.</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="8">
         <v>6408</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="8">
         <v>0</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="8">
         <v>5464</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="8">
         <v>10296</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="8">
         <v>7602</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="8">
         <v>4818</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="8">
         <v>34588</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="8">
         <v>6082</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="8">
+        <f t="shared" si="1"/>
         <v>40670</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="10">
         <v>16910.400000000001</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="10">
+        <f t="shared" si="2"/>
         <v>23759.599999999999</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="10">
         <v>22422.399999999998</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="10">
+        <f t="shared" si="3"/>
         <v>18247.600000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="85">
-      <c r="A7" s="4" t="str">
+    <row r="7" spans="1:18" ht="68">
+      <c r="A7" s="2" t="str">
         <f>_xlfn.CONCAT("A family with ", B7, " and ", D7, " would require $", M7, " to earn a living wage. Working at minimum wage would leave a gap of $", Q7, ". A family at the poverty level would need an additional $", O7, " to have the income required for a living wage.")</f>
         <v>A family with 2 adults and 1 child would require $49325 to earn a living wage. Working at minimum wage would leave a gap of $26902.6. A family at the poverty level would need an additional $28005 to have the income required for a living wage.</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="8">
         <v>7987</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="8">
         <v>0</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="8">
         <v>7033</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="8">
         <v>12072</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="8">
         <v>9644</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="8">
         <v>5003</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="8">
         <v>41738</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="8">
         <v>7586</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="8">
+        <f t="shared" si="1"/>
         <v>49325</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="10">
         <v>21320</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="10">
+        <f t="shared" si="2"/>
         <v>28005</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="10">
         <v>22422.399999999998</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="10">
+        <f t="shared" si="3"/>
         <v>26902.600000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="85">
-      <c r="A8" s="4" t="str">
+    <row r="8" spans="1:18" ht="68">
+      <c r="A8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>A family with 2 adults and 2 children would require $54866 to earn a living wage. Working at minimum wage would leave a gap of $32443.6. A family at the poverty level would need an additional $29115.6 to have the income required for a living wage.</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="8">
         <v>10303</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="8">
         <v>0</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="8">
         <v>7153</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="8">
         <v>12072</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="8">
         <v>10506</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="8">
         <v>6293</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="8">
         <v>46328</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="8">
         <v>8539</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="8">
+        <f t="shared" si="1"/>
         <v>54866</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="10">
         <v>25750.400000000001</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="10">
+        <f t="shared" si="2"/>
         <v>29115.599999999999</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="10">
         <v>22422.399999999998</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="10">
+        <f t="shared" si="3"/>
         <v>32443.600000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="85">
-      <c r="A9" s="4" t="str">
+    <row r="9" spans="1:18" ht="68">
+      <c r="A9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>A family with 2 adults and 3 children would require $61853 to earn a living wage. Working at minimum wage would leave a gap of $39430.6. A family at the poverty level would need an additional $31693 to have the income required for a living wage.</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="8">
         <v>12545</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="8">
         <v>0</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="8">
         <v>7055</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="8">
         <v>15144</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="8">
         <v>11013</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="8">
         <v>6296</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="8">
         <v>52052</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="8">
         <v>9800</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="8">
+        <f t="shared" si="1"/>
         <v>61853</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="10">
         <v>30160</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="10">
+        <f t="shared" si="2"/>
         <v>31693</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="10">
         <v>22422.399999999998</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="10">
+        <f t="shared" si="3"/>
         <v>39430.600000000006</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="85">
-      <c r="A10" s="4" t="str">
+      <c r="A10" s="2" t="str">
         <f>_xlfn.CONCAT("A family with ", B10, " and ", D10, " would require $", M10, " to earn a living wage. Working at minimum wage would provide a living wage with savings of $", Q10, ". A family at the poverty level would need an additional $", O10, " to have the income required for a living wage.")</f>
-        <v>A family with 2 adults and 0 children would require $40670 to earn a living wage. Working at minimum wage would provide a living wage with savings of $4174.8. A family at the poverty level would need an additional $23759.6 to have the income required for a living wage.</v>
-      </c>
-      <c r="B10" s="3" t="s">
+        <v>A family with 2 adults and 0 children would require $40670 to earn a living wage. Working at minimum wage would provide a living wage with savings of $4175. A family at the poverty level would need an additional $23759.6 to have the income required for a living wage.</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="8">
         <v>6408</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="9">
         <v>0</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="8">
         <v>5464</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="8">
         <v>10296</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="8">
         <v>7602</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="8">
         <v>4818</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="8">
         <v>34588</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="8">
         <v>6082</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="8">
+        <f t="shared" si="1"/>
         <v>40670</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="10">
         <v>16910.400000000001</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="10">
+        <f t="shared" si="2"/>
         <v>23759.599999999999</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="10">
         <v>44844.800000000003</v>
       </c>
-      <c r="Q10" s="7">
-        <f>P10-M10</f>
-        <v>4174.8000000000029</v>
+      <c r="Q10" s="10">
+        <v>4175</v>
       </c>
       <c r="R10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="85">
-      <c r="A11" s="4" t="str">
+    <row r="11" spans="1:18" ht="68">
+      <c r="A11" s="2" t="str">
         <f>_xlfn.CONCAT("A family with ", B11, " and ", D11, " would require $", M11, " to earn a living wage. Working at minimum wage would leave a gap of $", Q11, ". A family at the poverty level would need an additional $", O11, " to have the income required for a living wage.")</f>
-        <v>A family with 2 adults and 1 child would require $49325 to earn a living wage. Working at minimum wage would leave a gap of $4480.2. A family at the poverty level would need an additional $28005 to have the income required for a living wage.</v>
-      </c>
-      <c r="B11" s="3" t="s">
+        <v>A family with 2 adults and 1 child would require $58895.8 to earn a living wage. Working at minimum wage would leave a gap of $14051. A family at the poverty level would need an additional $37575.8 to have the income required for a living wage.</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="8">
         <v>7987</v>
       </c>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="F11" s="9">
+        <v>8235</v>
+      </c>
+      <c r="G11" s="8">
         <v>7033</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="8">
         <v>12072</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="8">
         <v>9644</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="8">
         <v>5003</v>
       </c>
-      <c r="K11" s="7">
-        <v>41738</v>
-      </c>
-      <c r="L11" s="7">
-        <v>7586</v>
-      </c>
-      <c r="M11" s="7">
-        <v>49325</v>
-      </c>
-      <c r="N11" s="6">
+      <c r="K11" s="8">
+        <f>M11-L11</f>
+        <v>49974</v>
+      </c>
+      <c r="L11" s="8">
+        <f>57560*0.155</f>
+        <v>8921.7999999999993</v>
+      </c>
+      <c r="M11" s="8">
+        <f t="shared" si="1"/>
+        <v>58895.8</v>
+      </c>
+      <c r="N11" s="10">
         <v>21320</v>
       </c>
-      <c r="O11" s="6">
-        <v>28005</v>
-      </c>
-      <c r="P11" s="6">
+      <c r="O11" s="10">
+        <f t="shared" si="2"/>
+        <v>37575.800000000003</v>
+      </c>
+      <c r="P11" s="10">
         <v>44844.800000000003</v>
       </c>
-      <c r="Q11" s="7">
-        <f t="shared" ref="Q11:Q13" si="1">M11 - P11</f>
-        <v>4480.1999999999971</v>
+      <c r="Q11" s="10">
+        <f t="shared" si="3"/>
+        <v>14051</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="85">
-      <c r="A12" s="4" t="str">
+      <c r="A12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>A family with 2 adults and 2 children would require $54866 to earn a living wage. Working at minimum wage would leave a gap of $10021.2. A family at the poverty level would need an additional $29115.6 to have the income required for a living wage.</v>
-      </c>
-      <c r="B12" s="3" t="s">
+        <v>A family with 2 adults and 2 children would require $68773.712 to earn a living wage. Working at minimum wage would leave a gap of $23928.912. A family at the poverty level would need an additional $43023.312 to have the income required for a living wage.</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="8">
         <v>10303</v>
       </c>
-      <c r="F12" s="7">
-        <v>0</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="F12" s="9">
+        <v>11898</v>
+      </c>
+      <c r="G12" s="8">
         <v>7153</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="8">
         <v>12072</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="8">
         <v>10506</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="8">
         <v>6293</v>
       </c>
-      <c r="K12" s="7">
-        <v>46328</v>
-      </c>
-      <c r="L12" s="7">
-        <v>8539</v>
-      </c>
-      <c r="M12" s="7">
-        <v>54866</v>
-      </c>
-      <c r="N12" s="6">
+      <c r="K12" s="8">
+        <f t="shared" ref="K12:K13" si="4">M12-L12</f>
+        <v>58225</v>
+      </c>
+      <c r="L12" s="8">
+        <f>66764*0.158</f>
+        <v>10548.712</v>
+      </c>
+      <c r="M12" s="8">
+        <f t="shared" si="1"/>
+        <v>68773.712</v>
+      </c>
+      <c r="N12" s="10">
         <v>25750.400000000001</v>
       </c>
-      <c r="O12" s="6">
-        <v>29115.599999999999</v>
-      </c>
-      <c r="P12" s="6">
+      <c r="O12" s="10">
+        <f t="shared" si="2"/>
+        <v>43023.311999999998</v>
+      </c>
+      <c r="P12" s="10">
         <v>44844.800000000003</v>
       </c>
-      <c r="Q12" s="7">
-        <f t="shared" si="1"/>
-        <v>10021.199999999997</v>
+      <c r="Q12" s="10">
+        <f t="shared" si="3"/>
+        <v>23928.911999999997</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="85">
-      <c r="A13" s="4" t="str">
+      <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>A family with 2 adults and 3 children would require $61853 to earn a living wage. Working at minimum wage would leave a gap of $17008.2. A family at the poverty level would need an additional $31693 to have the income required for a living wage.</v>
-      </c>
-      <c r="B13" s="3" t="s">
+        <v>A family with 2 adults and 3 children would require $80076.493 to earn a living wage. Working at minimum wage would leave a gap of $35231.693. A family at the poverty level would need an additional $49916.493 to have the income required for a living wage.</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="8">
         <v>12545</v>
       </c>
-      <c r="F13" s="7">
-        <v>0</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="F13" s="9">
+        <v>15560</v>
+      </c>
+      <c r="G13" s="8">
         <v>7055</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="8">
         <v>15144</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="8">
         <v>11013</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="8">
         <v>6296</v>
       </c>
-      <c r="K13" s="7">
-        <v>52052</v>
-      </c>
-      <c r="L13" s="7">
-        <v>9800</v>
-      </c>
-      <c r="M13" s="7">
-        <v>61853</v>
-      </c>
-      <c r="N13" s="6">
+      <c r="K13" s="8">
+        <f t="shared" si="4"/>
+        <v>67613</v>
+      </c>
+      <c r="L13" s="8">
+        <f>77413*0.161</f>
+        <v>12463.493</v>
+      </c>
+      <c r="M13" s="8">
+        <f t="shared" si="1"/>
+        <v>80076.493000000002</v>
+      </c>
+      <c r="N13" s="10">
         <v>30160</v>
       </c>
-      <c r="O13" s="6">
-        <v>31693</v>
-      </c>
-      <c r="P13" s="6">
+      <c r="O13" s="10">
+        <f t="shared" si="2"/>
+        <v>49916.493000000002</v>
+      </c>
+      <c r="P13" s="10">
         <v>44844.800000000003</v>
       </c>
-      <c r="Q13" s="7">
-        <f t="shared" si="1"/>
-        <v>17008.199999999997</v>
+      <c r="Q13" s="10">
+        <f t="shared" si="3"/>
+        <v>35231.692999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Format dollars for expenses
</commit_message>
<xml_diff>
--- a/addison_county_101/storymap_data/expenses_county.xlsx
+++ b/addison_county_101/storymap_data/expenses_county.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrence/Documents/GitHub/privilege_and_poverty/addison_county_101/storymap_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8BB877-C10F-9848-9BBF-E0DF9C3B57E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4475E9-A577-C246-955F-174F30AFD972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26860" yWindow="-860" windowWidth="34640" windowHeight="17240" xr2:uid="{F7A4D10A-304E-2D47-B0AF-70C3F3FAF73F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{F7A4D10A-304E-2D47-B0AF-70C3F3FAF73F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -597,8 +597,8 @@
     </row>
     <row r="2" spans="1:18" ht="68">
       <c r="A2" s="2" t="str">
-        <f>_xlfn.CONCAT("A family with ", B2, " and ", D2, " would require $", M2, " to earn a living wage. Working at minimum wage would leave a gap of $", Q2, ". A family at the poverty level would need an additional $", O2, " to have the income required for a living wage.")</f>
-        <v>A family with 1 adult and 0 children would require $24987 to earn a living wage. Working at minimum wage would leave a gap of $2564.6. A family at the poverty level would need an additional $12507 to have the income required for a living wage.</v>
+        <f>_xlfn.CONCAT("A family with ", B2, " and ", D2, " would require &lt;big&gt;&lt;b&gt;$", M2, "&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$", Q2, "&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$", O2, "&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.")</f>
+        <v>A family with 1 adult and 0 children would require &lt;big&gt;&lt;b&gt;$24987&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$2564.6&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$12507&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>16</v>
@@ -652,10 +652,10 @@
         <v>2564.6000000000022</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="68">
+    <row r="3" spans="1:18" ht="102">
       <c r="A3" s="2" t="str">
-        <f t="shared" ref="A3:A13" si="0">_xlfn.CONCAT("A family with ", B3, " and ", D3, " would require $", M3, " to earn a living wage. Working at minimum wage would leave a gap of $", Q3, ". A family at the poverty level would need an additional $", O3, " to have the income required for a living wage.")</f>
-        <v>A family with 1 adult and 1 child would require $53518 to earn a living wage. Working at minimum wage would leave a gap of $31095.6. A family at the poverty level would need an additional $36607.6 to have the income required for a living wage.</v>
+        <f t="shared" ref="A3:A13" si="0">_xlfn.CONCAT("A family with ", B3, " and ", D3, " would require &lt;big&gt;&lt;b&gt;$", M3, "&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$", Q3, "&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$", O3, "&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.")</f>
+        <v>A family with 1 adult and 1 child would require &lt;big&gt;&lt;b&gt;$53518&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$31095.6&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$36607.6&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>16</v>
@@ -709,10 +709,10 @@
         <v>31095.600000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="68">
+    <row r="4" spans="1:18" ht="102">
       <c r="A4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>A family with 1 adult and 2 children would require $63418 to earn a living wage. Working at minimum wage would leave a gap of $40995.6. A family at the poverty level would need an additional $42098 to have the income required for a living wage.</v>
+        <v>A family with 1 adult and 2 children would require &lt;big&gt;&lt;b&gt;$63418&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$40995.6&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$42098&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>16</v>
@@ -766,10 +766,10 @@
         <v>40995.600000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="68">
+    <row r="5" spans="1:18" ht="102">
       <c r="A5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>A family with 1 adult and 3 children would require $77424 to earn a living wage. Working at minimum wage would leave a gap of $55001.6. A family at the poverty level would need an additional $51673.6 to have the income required for a living wage.</v>
+        <v>A family with 1 adult and 3 children would require &lt;big&gt;&lt;b&gt;$77424&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$55001.6&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$51673.6&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>16</v>
@@ -823,10 +823,10 @@
         <v>55001.600000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="68">
+    <row r="6" spans="1:18" ht="102">
       <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>A family with 2 adults and 0 children would require $40670 to earn a living wage. Working at minimum wage would leave a gap of $18247.6. A family at the poverty level would need an additional $23759.6 to have the income required for a living wage.</v>
+        <v>A family with 2 adults and 0 children would require &lt;big&gt;&lt;b&gt;$40670&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$18247.6&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$23759.6&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>17</v>
@@ -880,10 +880,10 @@
         <v>18247.600000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="68">
+    <row r="7" spans="1:18" ht="102">
       <c r="A7" s="2" t="str">
-        <f>_xlfn.CONCAT("A family with ", B7, " and ", D7, " would require $", M7, " to earn a living wage. Working at minimum wage would leave a gap of $", Q7, ". A family at the poverty level would need an additional $", O7, " to have the income required for a living wage.")</f>
-        <v>A family with 2 adults and 1 child would require $49325 to earn a living wage. Working at minimum wage would leave a gap of $26902.6. A family at the poverty level would need an additional $28005 to have the income required for a living wage.</v>
+        <f t="shared" si="0"/>
+        <v>A family with 2 adults and 1 child would require &lt;big&gt;&lt;b&gt;$49325&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$26902.6&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$28005&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>17</v>
@@ -937,10 +937,10 @@
         <v>26902.600000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="68">
+    <row r="8" spans="1:18" ht="102">
       <c r="A8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>A family with 2 adults and 2 children would require $54866 to earn a living wage. Working at minimum wage would leave a gap of $32443.6. A family at the poverty level would need an additional $29115.6 to have the income required for a living wage.</v>
+        <v>A family with 2 adults and 2 children would require &lt;big&gt;&lt;b&gt;$54866&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$32443.6&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$29115.6&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>17</v>
@@ -994,10 +994,10 @@
         <v>32443.600000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="68">
+    <row r="9" spans="1:18" ht="102">
       <c r="A9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>A family with 2 adults and 3 children would require $61853 to earn a living wage. Working at minimum wage would leave a gap of $39430.6. A family at the poverty level would need an additional $31693 to have the income required for a living wage.</v>
+        <v>A family with 2 adults and 3 children would require &lt;big&gt;&lt;b&gt;$61853&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$39430.6&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$31693&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>17</v>
@@ -1051,10 +1051,10 @@
         <v>39430.600000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="85">
+    <row r="10" spans="1:18" ht="102">
       <c r="A10" s="2" t="str">
-        <f>_xlfn.CONCAT("A family with ", B10, " and ", D10, " would require $", M10, " to earn a living wage. Working at minimum wage would provide a living wage with savings of $", Q10, ". A family at the poverty level would need an additional $", O10, " to have the income required for a living wage.")</f>
-        <v>A family with 2 adults and 0 children would require $40670 to earn a living wage. Working at minimum wage would provide a living wage with savings of $4175. A family at the poverty level would need an additional $23759.6 to have the income required for a living wage.</v>
+        <f>_xlfn.CONCAT("A family with ", B10, " and ", D10, " would require &lt;big&gt;&lt;b&gt;$", M10, "&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would meet that level with &lt;big&gt;&lt;b&gt;&lt;i&gt;savings of $", Q10, "&lt;/i&gt;&lt;/b&gt;&lt;/big&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$", O10, "&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.")</f>
+        <v>A family with 2 adults and 0 children would require &lt;big&gt;&lt;b&gt;$40670&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would meet that level with &lt;big&gt;&lt;b&gt;&lt;i&gt;savings of $4175&lt;/i&gt;&lt;/b&gt;&lt;/big&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$23759.6&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>17</v>
@@ -1110,10 +1110,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="68">
+    <row r="11" spans="1:18" ht="102">
       <c r="A11" s="2" t="str">
-        <f>_xlfn.CONCAT("A family with ", B11, " and ", D11, " would require $", M11, " to earn a living wage. Working at minimum wage would leave a gap of $", Q11, ". A family at the poverty level would need an additional $", O11, " to have the income required for a living wage.")</f>
-        <v>A family with 2 adults and 1 child would require $58895.8 to earn a living wage. Working at minimum wage would leave a gap of $14051. A family at the poverty level would need an additional $37575.8 to have the income required for a living wage.</v>
+        <f t="shared" si="0"/>
+        <v>A family with 2 adults and 1 child would require &lt;big&gt;&lt;b&gt;$58895.8&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$14051&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$37575.8&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>17</v>
@@ -1169,10 +1169,10 @@
         <v>14051</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="85">
+    <row r="12" spans="1:18" ht="102">
       <c r="A12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>A family with 2 adults and 2 children would require $68773.712 to earn a living wage. Working at minimum wage would leave a gap of $23928.912. A family at the poverty level would need an additional $43023.312 to have the income required for a living wage.</v>
+        <v>A family with 2 adults and 2 children would require &lt;big&gt;&lt;b&gt;$68773.712&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$23928.912&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$43023.312&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>17</v>
@@ -1228,10 +1228,10 @@
         <v>23928.911999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="85">
+    <row r="13" spans="1:18" ht="102">
       <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>A family with 2 adults and 3 children would require $80076.493 to earn a living wage. Working at minimum wage would leave a gap of $35231.693. A family at the poverty level would need an additional $49916.493 to have the income required for a living wage.</v>
+        <v>A family with 2 adults and 3 children would require &lt;big&gt;&lt;b&gt;$80076.493&lt;/big&gt;&lt;/b&gt; to earn a living wage. Working at minimum wage would leave a gap of &lt;big&gt;&lt;b&gt;$35231.693&lt;/big&gt;&lt;/b&gt;. A family at the poverty level would need an additional &lt;big&gt;&lt;b&gt;$49916.493&lt;/big&gt;&lt;/b&gt; to have the income required for a living wage.</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Formats all dollars for expenses
</commit_message>
<xml_diff>
--- a/addison_county_101/storymap_data/expenses_county.xlsx
+++ b/addison_county_101/storymap_data/expenses_county.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrence/Documents/GitHub/privilege_and_poverty/addison_county_101/storymap_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4475E9-A577-C246-955F-174F30AFD972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED068CB-9717-C44A-8289-61851575E6DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{F7A4D10A-304E-2D47-B0AF-70C3F3FAF73F}"/>
   </bookViews>
@@ -517,9 +517,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A7FF57-4E4B-C441-9C00-37FB60C178BD}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>